<commit_message>
Code optimized and bug fixes
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,41 +470,142 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>is_anomaly</t>
+          <t>ERR1</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>anomaly</t>
+          <t>ERR2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ERR3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>192.168.1.1</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>44320.70833333334</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>192.168.1.2</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>44679.5</v>
-      </c>
-      <c r="C2" t="n">
-        <v>6</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="B3" s="2" t="n">
+        <v>44320.70980324074</v>
+      </c>
+      <c r="C3" t="n">
         <v>5</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>192.168.1.3</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>44320.71103009259</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>192.168.1.4</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>44320.72013888889</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>